<commit_message>
Wild type exceptions handled
</commit_message>
<xml_diff>
--- a/ref/Reportable_SNPs_Report_v2.xlsx
+++ b/ref/Reportable_SNPs_Report_v2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Eldin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\pyamd\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reportable_SNPs_PerPatient" sheetId="1" r:id="rId1"/>
@@ -213,130 +213,130 @@
     <t>Minor allele</t>
   </si>
   <si>
+    <t>37/81 (46)</t>
+  </si>
+  <si>
+    <t>42/81 (52)</t>
+  </si>
+  <si>
+    <t>2/81 (2)</t>
+  </si>
+  <si>
+    <t>81/81 (100)</t>
+  </si>
+  <si>
+    <t>0/81 (0)</t>
+  </si>
+  <si>
+    <t>36/81 (44)</t>
+  </si>
+  <si>
+    <t>43/81 (53)</t>
+  </si>
+  <si>
+    <t>38/81 (47)</t>
+  </si>
+  <si>
+    <t>41/81 (51)</t>
+  </si>
+  <si>
+    <t>59/81 (73)</t>
+  </si>
+  <si>
+    <t>19/81 (23)</t>
+  </si>
+  <si>
+    <t>3/81 (4)</t>
+  </si>
+  <si>
+    <t>64/81 (79)</t>
+  </si>
+  <si>
+    <t>14/81 (17)</t>
+  </si>
+  <si>
+    <t>35/81 (43)</t>
+  </si>
+  <si>
+    <t>40/81 (49)</t>
+  </si>
+  <si>
+    <t>6/81 (7)</t>
+  </si>
+  <si>
+    <t>80/81 (99)</t>
+  </si>
+  <si>
+    <t>1/81 (1)</t>
+  </si>
+  <si>
+    <t>79/81 (98)</t>
+  </si>
+  <si>
+    <t>76/81 (94)</t>
+  </si>
+  <si>
+    <t>5/81 (6)</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>K13</t>
+  </si>
+  <si>
+    <t>DHPS</t>
+  </si>
+  <si>
+    <t>45/81 (56)</t>
+  </si>
+  <si>
+    <t>30/81 (37)</t>
+  </si>
+  <si>
+    <t>72/81 (89)</t>
+  </si>
+  <si>
+    <t>9/81 (11)</t>
+  </si>
+  <si>
+    <t>70/81 (86)</t>
+  </si>
+  <si>
+    <t>10/81 (12)</t>
+  </si>
+  <si>
+    <t>60/81 (74)</t>
+  </si>
+  <si>
+    <t>18/81 (22)</t>
+  </si>
+  <si>
+    <t>DHFR</t>
+  </si>
+  <si>
+    <t>74/81 (91)</t>
+  </si>
+  <si>
+    <t>7/81 (9)</t>
+  </si>
+  <si>
+    <t>77/81 (95)</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
     <t>PfCRT</t>
   </si>
   <si>
-    <t>37/81 (46)</t>
-  </si>
-  <si>
-    <t>42/81 (52)</t>
-  </si>
-  <si>
-    <t>2/81 (2)</t>
-  </si>
-  <si>
-    <t>81/81 (100)</t>
-  </si>
-  <si>
-    <t>0/81 (0)</t>
-  </si>
-  <si>
-    <t>36/81 (44)</t>
-  </si>
-  <si>
-    <t>43/81 (53)</t>
-  </si>
-  <si>
-    <t>38/81 (47)</t>
-  </si>
-  <si>
-    <t>41/81 (51)</t>
-  </si>
-  <si>
-    <t>59/81 (73)</t>
-  </si>
-  <si>
-    <t>19/81 (23)</t>
-  </si>
-  <si>
-    <t>3/81 (4)</t>
-  </si>
-  <si>
     <t>PfMDR1</t>
-  </si>
-  <si>
-    <t>64/81 (79)</t>
-  </si>
-  <si>
-    <t>14/81 (17)</t>
-  </si>
-  <si>
-    <t>35/81 (43)</t>
-  </si>
-  <si>
-    <t>40/81 (49)</t>
-  </si>
-  <si>
-    <t>6/81 (7)</t>
-  </si>
-  <si>
-    <t>80/81 (99)</t>
-  </si>
-  <si>
-    <t>1/81 (1)</t>
-  </si>
-  <si>
-    <t>79/81 (98)</t>
-  </si>
-  <si>
-    <t>76/81 (94)</t>
-  </si>
-  <si>
-    <t>5/81 (6)</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>K13</t>
-  </si>
-  <si>
-    <t>DHPS</t>
-  </si>
-  <si>
-    <t>45/81 (56)</t>
-  </si>
-  <si>
-    <t>30/81 (37)</t>
-  </si>
-  <si>
-    <t>72/81 (89)</t>
-  </si>
-  <si>
-    <t>9/81 (11)</t>
-  </si>
-  <si>
-    <t>70/81 (86)</t>
-  </si>
-  <si>
-    <t>10/81 (12)</t>
-  </si>
-  <si>
-    <t>60/81 (74)</t>
-  </si>
-  <si>
-    <t>18/81 (22)</t>
-  </si>
-  <si>
-    <t>DHFR</t>
-  </si>
-  <si>
-    <t>74/81 (91)</t>
-  </si>
-  <si>
-    <t>7/81 (9)</t>
-  </si>
-  <si>
-    <t>77/81 (95)</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -378,6 +378,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -648,13 +651,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -677,7 +680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -826,7 +829,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5800</v>
       </c>
@@ -858,14 +861,14 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5801</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -877,13 +880,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>56</v>
       </c>
@@ -900,984 +903,984 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
         <v>62</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
         <v>67</v>
       </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
       <c r="F4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
         <v>69</v>
       </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
       <c r="F5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
         <v>62</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>63</v>
       </c>
-      <c r="F6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
         <v>71</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>72</v>
       </c>
-      <c r="F8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
         <v>62</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>63</v>
       </c>
-      <c r="F10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s">
         <v>77</v>
       </c>
-      <c r="E12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
         <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
         <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F35" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
         <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
         <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F41" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
         <v>48</v>
       </c>
       <c r="D43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F43" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
         <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
         <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
       </c>
       <c r="D46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F46" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C47" t="s">
         <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F47" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
         <v>53</v>
       </c>
       <c r="D48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F49" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
         <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F50" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DHPS:G437A changed to DHPS:A437G
</commit_message>
<xml_diff>
--- a/ref/Reportable_SNPs_Report_v2.xlsx
+++ b/ref/Reportable_SNPs_Report_v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="28800" windowHeight="17592" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reportable_SNPs_PerPatient" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="102">
   <si>
     <t>SampleID</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>PfMDR1</t>
+  </si>
+  <si>
+    <t>A437G</t>
   </si>
 </sst>
 </file>
@@ -655,9 +658,9 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -829,7 +832,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5800</v>
       </c>
@@ -861,12 +864,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5801</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -880,13 +883,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>56</v>
       </c>
@@ -903,7 +906,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -923,7 +926,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -943,7 +946,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -963,7 +966,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -983,7 +986,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1043,7 +1046,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1063,7 +1066,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1223,7 +1226,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1303,7 +1306,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1423,7 +1426,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1443,7 +1446,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1463,7 +1466,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1603,7 +1606,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1703,7 +1706,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
         <v>88</v>
@@ -1743,7 +1746,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1863,7 +1866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>

</xml_diff>